<commit_message>
Completed HashTable, Store, Hash and DataFile classes
</commit_message>
<xml_diff>
--- a/1- Perfect Hashing/Perfect Hashing/grocerystore.xlsx
+++ b/1- Perfect Hashing/Perfect Hashing/grocerystore.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Repos\knu-2nd\AlgorithmsAndComplexity\1- Perfect Hashing\Perfect Hashing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{76FCF2A7-09C7-403E-9377-4ACFEE0D72FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D1EA6D-CCD3-468E-BF64-F65610C544F6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20760" windowHeight="11055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20760" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Book1" sheetId="1" r:id="rId1"/>
@@ -20,22 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="48">
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>product</t>
-  </si>
-  <si>
-    <t>expiratin_date</t>
-  </si>
-  <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>cost</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
   <si>
     <t>fruits</t>
   </si>
@@ -169,7 +154,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -306,7 +291,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -484,12 +469,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -653,15 +632,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1016,11 +989,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,29 +1004,32 @@
     <col min="4" max="5" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>62</v>
@@ -1065,12 +1041,12 @@
         <v>6.03</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -1082,12 +1058,12 @@
         <v>12.53</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -1099,12 +1075,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>365</v>
@@ -1116,12 +1092,12 @@
         <v>11.73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
       <c r="C6">
         <v>16</v>
@@ -1133,12 +1109,12 @@
         <v>8.98</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>30</v>
@@ -1150,12 +1126,12 @@
         <v>7.33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -1167,12 +1143,12 @@
         <v>15.08</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>30</v>
@@ -1184,12 +1160,12 @@
         <v>9.44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>30</v>
@@ -1201,12 +1177,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>62</v>
@@ -1218,12 +1194,12 @@
         <v>15.66</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>90</v>
@@ -1235,12 +1211,12 @@
         <v>10.11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>90</v>
@@ -1252,12 +1228,12 @@
         <v>7.22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
       </c>
       <c r="C14">
         <v>90</v>
@@ -1269,12 +1245,12 @@
         <v>5.71</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>365</v>
@@ -1286,12 +1262,12 @@
         <v>4.7699999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>128</v>
@@ -1305,10 +1281,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <v>128</v>
@@ -1322,10 +1298,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>128</v>
@@ -1339,10 +1315,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>90</v>
@@ -1356,10 +1332,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>180</v>
@@ -1373,10 +1349,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>180</v>
@@ -1390,10 +1366,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C22">
         <v>180</v>
@@ -1407,10 +1383,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C23">
         <v>180</v>
@@ -1424,10 +1400,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>180</v>
@@ -1441,10 +1417,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
         <v>27</v>
-      </c>
-      <c r="B25" t="s">
-        <v>32</v>
       </c>
       <c r="C25">
         <v>180</v>
@@ -1458,10 +1434,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C26">
         <v>7</v>
@@ -1475,10 +1451,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C27">
         <v>16</v>
@@ -1492,10 +1468,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C28">
         <v>7</v>
@@ -1509,10 +1485,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C29">
         <v>16</v>
@@ -1526,10 +1502,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
         <v>33</v>
-      </c>
-      <c r="B30" t="s">
-        <v>38</v>
       </c>
       <c r="C30">
         <v>90</v>
@@ -1543,10 +1519,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C31">
         <v>90</v>
@@ -1560,10 +1536,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C32">
         <v>16</v>
@@ -1577,10 +1553,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C33">
         <v>90</v>
@@ -1594,10 +1570,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C34">
         <v>90</v>
@@ -1611,10 +1587,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C35">
         <v>365</v>
@@ -1628,10 +1604,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C36">
         <v>180</v>
@@ -1645,10 +1621,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C37">
         <v>90</v>
@@ -1662,10 +1638,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C38">
         <v>90</v>
@@ -1679,10 +1655,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C39">
         <v>7</v>

</xml_diff>